<commit_message>
authentication removed for report
</commit_message>
<xml_diff>
--- a/admin/controllers/thisMonthReport.xlsx
+++ b/admin/controllers/thisMonthReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Order ID</t>
   </si>
@@ -31,7 +31,7 @@
     <t>63e1d7198db3f87bb229bb25</t>
   </si>
   <si>
-    <t>Het Patel</t>
+    <t>Het B. Patel</t>
   </si>
   <si>
     <t>400</t>
@@ -41,6 +41,24 @@
   </si>
   <si>
     <t>KOT</t>
+  </si>
+  <si>
+    <t>63e22be88db3f87bb229bb74</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>63e22d478db3f87bb229bc52</t>
+  </si>
+  <si>
+    <t>Ayushi</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -86,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -126,6 +144,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
payment:complete online order added
</commit_message>
<xml_diff>
--- a/admin/controllers/thisMonthReport.xlsx
+++ b/admin/controllers/thisMonthReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Order ID</t>
   </si>
@@ -28,10 +28,22 @@
     <t>Payment Mode</t>
   </si>
   <si>
-    <t>63e1d7198db3f87bb229bb25</t>
+    <t>63e22be88db3f87bb229bb74</t>
   </si>
   <si>
-    <t>Het Patel</t>
+    <t>Het B. Patel</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>KOT</t>
+  </si>
+  <si>
+    <t>63e1d7198db3f87bb229bb25</t>
   </si>
   <si>
     <t>400</t>
@@ -40,7 +52,13 @@
     <t>2</t>
   </si>
   <si>
-    <t>KOT</t>
+    <t>63e22d478db3f87bb229bc52</t>
+  </si>
+  <si>
+    <t>Ayushi</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -86,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -126,6 +144,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>